<commit_message>
changes to patient requirements
</commit_message>
<xml_diff>
--- a/src/requirements/AipalCare Development Tasks.xlsx
+++ b/src/requirements/AipalCare Development Tasks.xlsx
@@ -1,30 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lordl\OneDrive\Documents\git\aipalcare-portal\src\requirements\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93286ABB-0672-4DE3-82C8-5BD642087738}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Requirements" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sprint-1" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Meeting notes" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Profile Requirements" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="TODO" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="DEV STAGES" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="Security" sheetId="7" r:id="rId10"/>
+    <sheet name="Requirements" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint-1" sheetId="2" r:id="rId2"/>
+    <sheet name="Meeting notes" sheetId="3" r:id="rId3"/>
+    <sheet name="Profile Requirements" sheetId="4" r:id="rId4"/>
+    <sheet name="TODO" sheetId="5" r:id="rId5"/>
+    <sheet name="DEV STAGES" sheetId="6" r:id="rId6"/>
+    <sheet name="Security" sheetId="7" r:id="rId7"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="C8">
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
-        <t xml:space="preserve">Is it possible to add an automatic reminder email 2 weeks before expiration?
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Is it possible to add an automatic reminder email 2 weeks before expiration?
 	-Maria Workman
 I don't think we can even have the clearance to capture Fingerprint, not sure of the laws around SSN storage as well, we need to find out.
 	-Aipal Care
@@ -33,6 +48,7 @@
 ----
 Can we add an automatic reminder 2 weeks before expiration date?
 	-Maria Workman</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -40,18 +56,25 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="C12">
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
-        <t xml:space="preserve">Be able to refer Patient
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Be able to refer Patient
 See Medical History - Records
 Evaluation
 Update Patient Records
 	-Aipal Care</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -59,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="132">
   <si>
     <t>Patient grants access to providers based on minimum required data - each medical info should be categorized and stored separately</t>
   </si>
@@ -304,6 +327,8 @@
     <r>
       <rPr>
         <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>therapist/staff</t>
     </r>
@@ -439,38 +464,80 @@
   </si>
   <si>
     <t>Data Security at rest</t>
+  </si>
+  <si>
+    <t>Patient Registration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Patient: </t>
+  </si>
+  <si>
+    <t>First Name, Last Name of patient, birth date, photo</t>
+  </si>
+  <si>
+    <t>First Name, Last Name, phone number, email address, home address of primary guardian (insurance coverage), relationship</t>
+  </si>
+  <si>
+    <t>First Name, Last Name, phone number, email address, home address of secondary guardian</t>
+  </si>
+  <si>
+    <t>Primary Care Physician, Practice Name, phone number, fax number, NPI number</t>
+  </si>
+  <si>
+    <t>Insurance, insurance verification, copay</t>
+  </si>
+  <si>
+    <t>Therapy recommendation:  30 minute sessions, xper week, for 12 weeks, progress note due date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m-d"/>
+    <numFmt numFmtId="164" formatCode="m\-d"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -478,7 +545,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -506,191 +573,153 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="22">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE0F7FA"/>
+          <bgColor rgb="FFE0F7FA"/>
+        </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4DD0E1"/>
+          <bgColor rgb="FF4DD0E1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFBDBDBD"/>
           <bgColor rgb="FFBDBDBD"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF3F3F3"/>
-          <bgColor rgb="FFF3F3F3"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF4DD0E1"/>
-          <bgColor rgb="FF4DD0E1"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE0F7FA"/>
-          <bgColor rgb="FFE0F7FA"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="2">
-    <tableStyle count="3" pivot="0" name="Profile Requirements-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    <tableStyle name="Profile Requirements-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="firstRowStripe" dxfId="4"/>
+      <tableStyleElement type="secondRowStripe" dxfId="3"/>
     </tableStyle>
-    <tableStyle count="3" pivot="0" name="Profile Requirements-style 2">
-      <tableStyleElement dxfId="4" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="5" type="secondRowStripe"/>
+    <tableStyle name="Profile Requirements-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B8:D13" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="B8:D13">
   <tableColumns count="3">
-    <tableColumn name="FBI Fingerprinting Clearance" id="1"/>
-    <tableColumn name="-expiration date" id="2"/>
-    <tableColumn name="-place to upload document" id="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="FBI Fingerprinting Clearance"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="-expiration date"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="-place to upload document"/>
   </tableColumns>
-  <tableStyleInfo name="Profile Requirements-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Profile Requirements-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A2:C7" displayName="Table_2" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="A2:C7">
   <tableColumns count="3">
-    <tableColumn name="Organization" id="1"/>
-    <tableColumn name="Name, Credentials, License Number and National Health Provider Number of Primary Health Provider" id="2"/>
-    <tableColumn name="Credit card number, Name as it appears on card, Expiration date, Billing zip code," id="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Organization"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name, Credentials, License Number and National Health Provider Number of Primary Health Provider"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Credit card number, Name as it appears on card, Expiration date, Billing zip code,"/>
   </tableColumns>
-  <tableStyleInfo name="Profile Requirements-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Profile Requirements-style 2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -880,43 +909,46 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="50.86"/>
-    <col customWidth="1" min="2" max="2" width="101.29"/>
-    <col customWidth="1" min="3" max="3" width="33.86"/>
-    <col customWidth="1" min="4" max="4" width="29.57"/>
-    <col customWidth="1" min="5" max="5" width="22.86"/>
-    <col customWidth="1" min="6" max="6" width="26.71"/>
+    <col min="1" max="1" width="50.85546875" customWidth="1"/>
+    <col min="2" max="2" width="101.28515625" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -934,12 +966,12 @@
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -947,7 +979,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
@@ -955,12 +987,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
@@ -974,7 +1006,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -991,120 +1023,122 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="43.86"/>
-    <col customWidth="1" min="2" max="2" width="20.14"/>
+    <col min="1" max="1" width="43.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
@@ -1112,38 +1146,41 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:B23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.86"/>
-    <col customWidth="1" min="2" max="2" width="62.29"/>
-    <col customWidth="1" min="3" max="3" width="50.86"/>
-    <col customWidth="1" min="4" max="4" width="43.0"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="106.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" customWidth="1"/>
+    <col min="4" max="4" width="43" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>43</v>
       </c>
@@ -1154,7 +1191,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>46</v>
       </c>
@@ -1163,14 +1200,14 @@
       </c>
       <c r="C3" s="7"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C4" s="7"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
       <c r="B5" s="4" t="s">
         <v>49</v>
@@ -1179,21 +1216,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="7"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
       <c r="B7" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C7" s="7"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
         <v>53</v>
       </c>
@@ -1204,7 +1241,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
         <v>56</v>
       </c>
@@ -1215,7 +1252,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
         <v>57</v>
       </c>
@@ -1226,7 +1263,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
         <v>58</v>
       </c>
@@ -1237,7 +1274,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="s">
         <v>59</v>
       </c>
@@ -1248,7 +1285,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
         <v>60</v>
       </c>
@@ -1257,30 +1294,73 @@
       </c>
       <c r="D13" s="10"/>
     </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="21"/>
+    </row>
+    <row r="18" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="21" t="s">
+        <v>131</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="2">
-    <tablePart r:id="rId6"/>
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="130.57"/>
+    <col min="1" max="1" width="130.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>61</v>
       </c>
@@ -1288,7 +1368,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>63</v>
       </c>
@@ -1296,83 +1376,84 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>74</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AA37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="71.29"/>
-    <col customWidth="1" min="2" max="2" width="31.86"/>
-    <col customWidth="1" min="3" max="4" width="34.0"/>
-    <col customWidth="1" min="5" max="5" width="29.71"/>
-    <col customWidth="1" min="6" max="6" width="23.0"/>
-    <col customWidth="1" min="8" max="8" width="41.43"/>
+    <col min="1" max="1" width="71.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="3" max="4" width="34" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="8" max="8" width="41.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>75</v>
       </c>
@@ -1399,7 +1480,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>83</v>
       </c>
@@ -1411,7 +1492,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>86</v>
       </c>
@@ -1426,12 +1507,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>91</v>
       </c>
@@ -1439,7 +1520,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>93</v>
       </c>
@@ -1447,14 +1528,15 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B10" s="13"/>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="19" t="s">
         <v>96</v>
       </c>
+      <c r="D10" s="20"/>
       <c r="E10" s="14"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
@@ -1462,7 +1544,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" s="14"/>
       <c r="C11" s="15" t="s">
         <v>98</v>
@@ -1475,9 +1557,9 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" s="16">
-        <v>44052.0</v>
+        <v>44052</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>100</v>
@@ -1490,9 +1572,9 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" s="16">
-        <v>43832.0</v>
+        <v>43832</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -1501,7 +1583,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -1510,7 +1592,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
@@ -1519,7 +1601,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>102</v>
       </c>
@@ -1531,7 +1613,7 @@
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>103</v>
       </c>
@@ -1543,7 +1625,7 @@
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>104</v>
       </c>
@@ -1551,12 +1633,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>107</v>
       </c>
@@ -1568,22 +1650,22 @@
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>113</v>
       </c>
@@ -1614,22 +1696,22 @@
       <c r="Z30" s="18"/>
       <c r="AA30" s="18"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>117</v>
       </c>
@@ -1638,55 +1720,56 @@
   <mergeCells count="1">
     <mergeCell ref="C10:D10"/>
   </mergeCells>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="58.0"/>
+    <col min="1" max="1" width="58" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>123</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>